<commit_message>
Fixed bug with subscription cancel mailer
</commit_message>
<xml_diff>
--- a/TestingPlan.xlsx
+++ b/TestingPlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-18.04\home\ryan\Ruby\RubyWebsite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C9601B-2742-4C93-B8C9-798A5C983065}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{646BB6DF-0550-4BAE-8429-42B7AC215FEC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{7A891BF7-FC02-40A4-AEEE-78F6C58F7248}"/>
+    <workbookView xWindow="7725" yWindow="4515" windowWidth="28800" windowHeight="15300" xr2:uid="{7A891BF7-FC02-40A4-AEEE-78F6C58F7248}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="54">
   <si>
     <t>Test Number</t>
   </si>
@@ -211,91 +211,6 @@
 3. Verify a popup is displayed, then click ok
 4. Verify the vehicle is removed but all the other buttons are enabled
 5. Check that the order option for that vehicle has been removed from the DB</t>
-  </si>
-  <si>
-    <t>2-1</t>
-  </si>
-  <si>
-    <t>2-2</t>
-  </si>
-  <si>
-    <t>2-3</t>
-  </si>
-  <si>
-    <t>2-4</t>
-  </si>
-  <si>
-    <t>2-5</t>
-  </si>
-  <si>
-    <t>2-6</t>
-  </si>
-  <si>
-    <t>2-7</t>
-  </si>
-  <si>
-    <t>2-8</t>
-  </si>
-  <si>
-    <t>2-9</t>
-  </si>
-  <si>
-    <t>2-10</t>
-  </si>
-  <si>
-    <t>2-11</t>
-  </si>
-  <si>
-    <t>2-12</t>
-  </si>
-  <si>
-    <t>2-13</t>
-  </si>
-  <si>
-    <t>2-14</t>
-  </si>
-  <si>
-    <t>2-15</t>
-  </si>
-  <si>
-    <t>2-16</t>
-  </si>
-  <si>
-    <t>2-17</t>
-  </si>
-  <si>
-    <t>2-18</t>
-  </si>
-  <si>
-    <t>2-19</t>
-  </si>
-  <si>
-    <t>2-20</t>
-  </si>
-  <si>
-    <t>2-21</t>
-  </si>
-  <si>
-    <t>Shipping Charge</t>
-  </si>
-  <si>
-    <t>Existing account</t>
-  </si>
-  <si>
-    <t>Shipping charged on all new orders</t>
-  </si>
-  <si>
-    <t>Shipping is not charged on first subscription</t>
-  </si>
-  <si>
-    <t>1. Add a new subscription to an existing account
-2. Verify that in the Stripe invoice, the customer was charged for shipping
-3. Verify that the shipping included flag is true in the database</t>
-  </si>
-  <si>
-    <t>1. Create a new subscription
-2. Verify that in the Stripe invoice, the customer was not charged for shipping
-3. Verify in the DB that the shipping included flag is false for all the orders created</t>
   </si>
 </sst>
 </file>
@@ -673,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB24EEBE-C504-4326-9FFB-0C6707DE6742}">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +931,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>35</v>
       </c>
@@ -1024,141 +939,12 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A37" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>